<commit_message>
Add: 1/5 of functions added
</commit_message>
<xml_diff>
--- a/inst/extdata/input/Environment_Sheet.xlsx
+++ b/inst/extdata/input/Environment_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCE0B8E-2639-4620-A952-E56EDA3654CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1481CF3A-3EB3-4461-ACEB-9BB25864451E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="560" windowWidth="9320" windowHeight="8360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>k_aslAir</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>k_aslSoilAir</t>
   </si>
   <si>
@@ -79,12 +76,6 @@
     <t>f_water</t>
   </si>
   <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Distribution</t>
-  </si>
-  <si>
     <t>see the sheets "Parameters" and "Distributions"</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
   </si>
   <si>
     <t>%</t>
-  </si>
-  <si>
-    <t>Parameter</t>
   </si>
   <si>
     <t>none</t>
@@ -243,12 +231,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Value_1</t>
-  </si>
-  <si>
-    <t>Value_2</t>
-  </si>
-  <si>
     <t>f_resorbed</t>
   </si>
   <si>
@@ -328,6 +310,24 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>value_1</t>
+  </si>
+  <si>
+    <t>value_2</t>
+  </si>
+  <si>
+    <t>distribution</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
 </sst>
 </file>
@@ -785,7 +785,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,28 +798,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -828,107 +828,107 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4">
         <v>120</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4">
         <v>0.48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5">
         <v>4.8000000000000001E-5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D5" s="4">
         <v>8.3144589999999994</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2">
         <v>0.2</v>
@@ -938,21 +938,21 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2">
         <v>0.2</v>
@@ -962,21 +962,21 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>0.6</v>
@@ -986,21 +986,21 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
         <v>-3.9330381952821201</v>
@@ -1012,47 +1012,47 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>2500</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2">
         <v>1700</v>
@@ -1062,47 +1062,47 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2">
         <v>0.2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2">
         <v>5</v>
@@ -1114,21 +1114,21 @@
         <v>0</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2">
         <v>0.25</v>
@@ -1138,21 +1138,21 @@
         <v>0</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="3">
         <v>283.2</v>
@@ -1162,21 +1162,21 @@
         <v>0</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3">
         <v>1.8083544581018101</v>
@@ -1188,47 +1188,47 @@
         <v>1.2473438276712301E-3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D17" s="3">
         <v>180</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3">
         <v>0.8</v>
@@ -1238,47 +1238,47 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D19" s="3">
         <v>86</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3">
         <v>60</v>
@@ -1290,99 +1290,99 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3">
         <v>0.15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D22" s="3">
         <v>0.5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3">
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
@@ -1394,21 +1394,21 @@
         <v>0</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D25" s="8">
         <v>5.9367998000000002</v>
@@ -1420,36 +1420,36 @@
         <v>0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1471,12 +1471,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify data loading and preparation
</commit_message>
<xml_diff>
--- a/inst/extdata/input/Environment_Sheet.xlsx
+++ b/inst/extdata/input/Environment_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1481CF3A-3EB3-4461-ACEB-9BB25864451E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FDA4A-A648-416F-851D-1BF58F588984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="560" windowWidth="9320" windowHeight="8360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
   <si>
     <t>k_aslAir</t>
   </si>
@@ -181,53 +181,6 @@
     <t>plant dry mass</t>
   </si>
   <si>
-    <r>
-      <t>kg P</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/(ha*a)</t>
-    </r>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -276,9 +229,6 @@
     <t>p_app</t>
   </si>
   <si>
-    <t>yearly P2O5 application</t>
-  </si>
-  <si>
     <t>normal</t>
   </si>
   <si>
@@ -328,22 +278,26 @@
   </si>
   <si>
     <t>unit</t>
+  </si>
+  <si>
+    <t>yearly fertilizer application</t>
+  </si>
+  <si>
+    <t>kg /(ha*a)</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -782,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,35 +748,44 @@
     <col min="2" max="2" width="40.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6328125" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.08984375" customWidth="1"/>
+    <col min="10" max="10" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -834,7 +797,7 @@
         <v>120</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -843,10 +806,12 @@
         <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -858,7 +823,7 @@
         <v>0.48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -867,10 +832,12 @@
         <v>25</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -882,7 +849,7 @@
         <v>4.8000000000000001E-5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -891,10 +858,12 @@
         <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -902,13 +871,13 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="4">
         <v>8.3144589999999994</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -917,10 +886,12 @@
         <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -941,10 +912,12 @@
         <v>25</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -965,10 +938,12 @@
         <v>25</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -989,10 +964,12 @@
         <v>25</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1012,13 +989,15 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1011,7 @@
         <v>2500</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1041,10 +1020,12 @@
         <v>25</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1065,10 +1046,12 @@
         <v>25</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1082,7 +1065,7 @@
         <v>0.2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
@@ -1091,15 +1074,17 @@
         <v>25</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -1114,13 +1099,15 @@
         <v>0</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1141,10 +1128,12 @@
         <v>25</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1165,10 +1154,12 @@
         <v>25</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1188,13 +1179,15 @@
         <v>1.2473438276712301E-3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1201,7 @@
         <v>180</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1217,10 +1210,12 @@
         <v>25</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1241,10 +1236,12 @@
         <v>25</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1258,50 +1255,55 @@
         <v>86</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="3">
+        <v>750</v>
+      </c>
+      <c r="E20" s="1">
+        <f>10/60*750</f>
+        <v>125</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="3">
-        <v>60</v>
-      </c>
-      <c r="E20" s="1">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>19</v>
@@ -1310,7 +1312,7 @@
         <v>0.15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1319,15 +1321,17 @@
         <v>25</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>19</v>
@@ -1336,7 +1340,7 @@
         <v>0.5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1345,24 +1349,26 @@
         <v>25</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D23" s="3">
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1371,18 +1377,20 @@
         <v>25</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
@@ -1394,18 +1402,20 @@
         <v>0</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>21</v>
@@ -1420,18 +1430,20 @@
         <v>0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>21</v>
@@ -1440,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
@@ -1449,8 +1461,10 @@
         <v>25</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>69</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Add PEC calculation functions
</commit_message>
<xml_diff>
--- a/inst/extdata/input/Environment_Sheet.xlsx
+++ b/inst/extdata/input/Environment_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FDA4A-A648-416F-851D-1BF58F588984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7127B412-64C4-4C1D-A6FA-4B7433B76629}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="560" windowWidth="9320" windowHeight="8360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
   <si>
     <t>k_aslAir</t>
   </si>
@@ -196,9 +196,6 @@
     <t>fraction of substance intake via food</t>
   </si>
   <si>
-    <t>m_wheat</t>
-  </si>
-  <si>
     <t>consumption of wheat per day</t>
   </si>
   <si>
@@ -290,6 +287,12 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>Wheat consumption</t>
+  </si>
+  <si>
+    <t>m_crop</t>
   </si>
 </sst>
 </file>
@@ -738,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,34 +758,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -806,7 +809,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -832,7 +835,7 @@
         <v>25</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -858,7 +861,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -871,7 +874,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="4">
         <v>8.3144589999999994</v>
@@ -886,7 +889,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -912,7 +915,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -938,7 +941,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -964,7 +967,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -989,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1020,7 +1023,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1046,7 +1049,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1074,17 +1077,17 @@
         <v>25</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -1099,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1128,7 +1131,7 @@
         <v>25</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1154,7 +1157,7 @@
         <v>25</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1179,10 +1182,10 @@
         <v>1.2473438276712301E-3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1210,7 +1213,7 @@
         <v>25</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1236,7 +1239,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1264,20 +1267,20 @@
         <v>25</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D20" s="3">
         <v>750</v>
@@ -1290,10 +1293,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1321,7 +1324,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1349,20 +1352,20 @@
         <v>25</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D23" s="3">
         <v>600</v>
@@ -1377,20 +1380,22 @@
         <v>25</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
@@ -1402,20 +1407,20 @@
         <v>0</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>21</v>
@@ -1430,20 +1435,20 @@
         <v>0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>21</v>
@@ -1461,7 +1466,7 @@
         <v>25</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>

</xml_diff>

<commit_message>
Mod: Fertilizer application moved to substance sheet
This was the only line in the environmental sheet that depended on the fertilizer type and not on the environment. --> Moved to substance sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/input/Environment_Sheet.xlsx
+++ b/inst/extdata/input/Environment_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7127B412-64C4-4C1D-A6FA-4B7433B76629}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE75D2F5-793F-49CA-B8EB-DFF2FAFB9EF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="560" windowWidth="9320" windowHeight="8360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
   <si>
     <t>k_aslAir</t>
   </si>
@@ -223,12 +223,6 @@
     <t>(kg*m²)/(s²mol*K)</t>
   </si>
   <si>
-    <t>p_app</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
     <t>v_G</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>site_specific</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
@@ -275,12 +266,6 @@
   </si>
   <si>
     <t>unit</t>
-  </si>
-  <si>
-    <t>yearly fertilizer application</t>
-  </si>
-  <si>
-    <t>kg /(ha*a)</t>
   </si>
   <si>
     <t>references</t>
@@ -739,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,34 +743,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>50</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -809,7 +794,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -835,7 +820,7 @@
         <v>25</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -861,7 +846,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -889,7 +874,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -915,7 +900,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -941,7 +926,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -967,7 +952,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -995,7 +980,7 @@
         <v>53</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1023,7 +1008,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1049,7 +1034,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1077,7 +1062,7 @@
         <v>25</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1105,7 +1090,7 @@
         <v>52</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1131,7 +1116,7 @@
         <v>25</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1157,7 +1142,7 @@
         <v>25</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1185,7 +1170,7 @@
         <v>51</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1213,7 +1198,7 @@
         <v>25</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1239,7 +1224,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1267,52 +1252,51 @@
         <v>25</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="D20" s="3">
-        <v>750</v>
-      </c>
-      <c r="E20" s="1">
-        <f>10/60*750</f>
-        <v>125</v>
+        <v>0.15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="3">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>41</v>
@@ -1324,23 +1308,23 @@
         <v>25</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3">
-        <v>0.5</v>
+        <v>600</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
@@ -1352,65 +1336,65 @@
         <v>25</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="3">
-        <v>600</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>25</v>
+      <c r="A23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D24" s="8">
-        <v>1</v>
+        <v>5.9367998000000002</v>
       </c>
       <c r="E24" s="1">
-        <v>1000</v>
+        <v>0.80589460000000002</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1426,50 +1410,22 @@
         <v>21</v>
       </c>
       <c r="D25" s="8">
-        <v>5.9367998000000002</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0.80589460000000002</v>
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="8">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>